<commit_message>
Chunk Numbering Chaged. Other improvements. Ongoing 303
</commit_message>
<xml_diff>
--- a/data/aa.xlsx
+++ b/data/aa.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Analytics\xADSM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526EE3CD-4097-42FB-A98C-98DE95CDF985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F5C0F9-A2A9-4005-A5D4-9FE400DDE848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="-110" windowWidth="18440" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="-110" windowWidth="18440" windowHeight="11020" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
     <sheet name="bb" sheetId="1" r:id="rId3"/>
-    <sheet name="BE01" sheetId="2" r:id="rId4"/>
-    <sheet name="IN" sheetId="7" r:id="rId5"/>
-    <sheet name="ConCat" sheetId="8" r:id="rId6"/>
-    <sheet name="PipeCat" sheetId="9" r:id="rId7"/>
+    <sheet name="IN" sheetId="7" r:id="rId4"/>
+    <sheet name="ConCat" sheetId="8" r:id="rId5"/>
+    <sheet name="PipeCat" sheetId="9" r:id="rId6"/>
+    <sheet name="BE01" sheetId="2" r:id="rId7"/>
+    <sheet name="BE02" sheetId="10" r:id="rId8"/>
+    <sheet name="BE03" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="R_Sep">IN!$A$1</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="148">
   <si>
     <t>xx</t>
   </si>
@@ -417,6 +419,78 @@
   </si>
   <si>
     <t>100 (85%)</t>
+  </si>
+  <si>
+    <t>Soft_Drink</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Diet Coke</t>
+  </si>
+  <si>
+    <t>Dr. Pepper</t>
+  </si>
+  <si>
+    <t>Judge_Case</t>
+  </si>
+  <si>
+    <t>Luckett</t>
+  </si>
+  <si>
+    <t>Kendall</t>
+  </si>
+  <si>
+    <t>Common Pleas</t>
+  </si>
+  <si>
+    <t>Municipal Court</t>
+  </si>
+  <si>
+    <t>Ex27</t>
+  </si>
+  <si>
+    <t>Ex28</t>
+  </si>
+  <si>
+    <t>BE0214</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Commercials</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Purchase</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Cost_per_kg</t>
   </si>
 </sst>
 </file>
@@ -1322,614 +1396,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{634B976E-6278-4D6D-8D44-5D014C68FAE9}">
-  <dimension ref="A1:K30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3">
-        <v>60</v>
-      </c>
-      <c r="E3">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>80</v>
-      </c>
-      <c r="E4">
-        <v>70</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5">
-        <v>78</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6">
-        <v>70</v>
-      </c>
-      <c r="E6">
-        <v>72</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7">
-        <v>45</v>
-      </c>
-      <c r="E7">
-        <v>70</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8">
-        <v>80</v>
-      </c>
-      <c r="E8">
-        <v>73</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9">
-        <v>60</v>
-      </c>
-      <c r="E9">
-        <v>72</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10">
-        <v>50</v>
-      </c>
-      <c r="E10">
-        <v>72</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="4">
-        <v>599</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="1">
-        <v>10.1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="4">
-        <v>299</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="F15" s="1">
-        <v>9</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="4">
-        <v>499</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="1">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="F16" s="1">
-        <v>11</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>4</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="4">
-        <v>860</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="1">
-        <v>11.6</v>
-      </c>
-      <c r="F17" s="1">
-        <v>8</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>5</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="4">
-        <v>668</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="1">
-        <v>10.1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>10.5</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>6</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="4">
-        <v>899</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="1">
-        <v>10.6</v>
-      </c>
-      <c r="F19" s="1">
-        <v>4</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
-        <v>7</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="4">
-        <v>530</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="1">
-        <v>10.1</v>
-      </c>
-      <c r="F20" s="1">
-        <v>9</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
-        <v>8</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="4">
-        <v>590</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="1">
-        <v>11.6</v>
-      </c>
-      <c r="F21" s="1">
-        <v>7</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
-        <v>9</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="4">
-        <v>525</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="1">
-        <v>10.1</v>
-      </c>
-      <c r="F22" s="1">
-        <v>10</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
-        <v>10</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="4">
-        <v>360</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="1">
-        <v>9.4</v>
-      </c>
-      <c r="F23" s="1">
-        <v>8</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B26" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" s="11">
-        <v>2007</v>
-      </c>
-      <c r="D26" s="11">
-        <v>2008</v>
-      </c>
-      <c r="E26" s="11">
-        <v>2009</v>
-      </c>
-      <c r="F26" s="11">
-        <v>2010</v>
-      </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B27" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27">
-        <v>327</v>
-      </c>
-      <c r="D27">
-        <v>311</v>
-      </c>
-      <c r="E27">
-        <v>286</v>
-      </c>
-      <c r="F27">
-        <v>290</v>
-      </c>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B28" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28">
-        <v>167</v>
-      </c>
-      <c r="D28">
-        <v>140</v>
-      </c>
-      <c r="E28">
-        <v>106</v>
-      </c>
-      <c r="F28">
-        <v>108</v>
-      </c>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B29" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29">
-        <v>204</v>
-      </c>
-      <c r="D29">
-        <v>220</v>
-      </c>
-      <c r="E29">
-        <v>300</v>
-      </c>
-      <c r="F29">
-        <v>270</v>
-      </c>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="H30" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8725100-A1E1-4BF5-A8F9-DEA8ACC33E0A}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -2072,7 +1538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA66420-FCC3-4F4D-876A-FF97C28DB8E8}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -2177,7 +1643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C338BD5C-8F45-426F-A26F-2CE0AF58B2C7}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -2280,4 +1746,1522 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{634B976E-6278-4D6D-8D44-5D014C68FAE9}">
+  <dimension ref="A1:K30"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>70</v>
+      </c>
+      <c r="E6">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+      <c r="E7">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="4">
+        <v>599</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="4">
+        <v>299</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="F15" s="1">
+        <v>9</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="4">
+        <v>499</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F16" s="1">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="4">
+        <v>860</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="F17" s="1">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="4">
+        <v>668</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="4">
+        <v>899</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>7</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="4">
+        <v>530</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="4">
+        <v>590</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="F21" s="1">
+        <v>7</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="4">
+        <v>525</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="4">
+        <v>360</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="F23" s="1">
+        <v>8</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B26" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="11">
+        <v>2007</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2008</v>
+      </c>
+      <c r="E26" s="11">
+        <v>2009</v>
+      </c>
+      <c r="F26" s="11">
+        <v>2010</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B27" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27">
+        <v>327</v>
+      </c>
+      <c r="D27">
+        <v>311</v>
+      </c>
+      <c r="E27">
+        <v>286</v>
+      </c>
+      <c r="F27">
+        <v>290</v>
+      </c>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B28" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28">
+        <v>167</v>
+      </c>
+      <c r="D28">
+        <v>140</v>
+      </c>
+      <c r="E28">
+        <v>106</v>
+      </c>
+      <c r="F28">
+        <v>108</v>
+      </c>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B29" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29">
+        <v>204</v>
+      </c>
+      <c r="D29">
+        <v>220</v>
+      </c>
+      <c r="E29">
+        <v>300</v>
+      </c>
+      <c r="F29">
+        <v>270</v>
+      </c>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H30" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CB65A3-1364-407C-A218-9CEDDB8B50CA}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9">
+        <v>129</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9">
+        <v>29</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9">
+        <v>90</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10">
+        <v>110</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10">
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="11">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>28</v>
+      </c>
+      <c r="G14">
+        <v>72</v>
+      </c>
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="11">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>17</v>
+      </c>
+      <c r="G15">
+        <v>99</v>
+      </c>
+      <c r="I15" s="11">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="11">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>52</v>
+      </c>
+      <c r="G16">
+        <v>58</v>
+      </c>
+      <c r="I16" s="11">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="11">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>79</v>
+      </c>
+      <c r="G17">
+        <v>34</v>
+      </c>
+      <c r="I17" s="11">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="11">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>37</v>
+      </c>
+      <c r="G18">
+        <v>60</v>
+      </c>
+      <c r="I18" s="11">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="11">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="11">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>71</v>
+      </c>
+      <c r="G19">
+        <v>22</v>
+      </c>
+      <c r="I19" s="11">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="11">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="11">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>37</v>
+      </c>
+      <c r="G20">
+        <v>77</v>
+      </c>
+      <c r="I20" s="11">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="11">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="11">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>27</v>
+      </c>
+      <c r="G21">
+        <v>85</v>
+      </c>
+      <c r="I21" s="11">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="11">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="11">
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <v>64</v>
+      </c>
+      <c r="G22">
+        <v>45</v>
+      </c>
+      <c r="I22" s="11">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="11">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="11">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>53</v>
+      </c>
+      <c r="G23">
+        <v>47</v>
+      </c>
+      <c r="I23" s="11">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="11">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="11">
+        <v>11</v>
+      </c>
+      <c r="F24">
+        <v>13</v>
+      </c>
+      <c r="G24">
+        <v>98</v>
+      </c>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="11">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11">
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>84</v>
+      </c>
+      <c r="G25">
+        <v>21</v>
+      </c>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="11">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="E26" s="11">
+        <v>13</v>
+      </c>
+      <c r="F26">
+        <v>59</v>
+      </c>
+      <c r="G26">
+        <v>32</v>
+      </c>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="11">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="E27" s="11">
+        <v>14</v>
+      </c>
+      <c r="F27">
+        <v>17</v>
+      </c>
+      <c r="G27">
+        <v>81</v>
+      </c>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="11">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="E28" s="11">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>70</v>
+      </c>
+      <c r="G28">
+        <v>34</v>
+      </c>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="11">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="E29" s="11">
+        <v>16</v>
+      </c>
+      <c r="F29">
+        <v>47</v>
+      </c>
+      <c r="G29">
+        <v>64</v>
+      </c>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="11">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="11">
+        <v>17</v>
+      </c>
+      <c r="F30">
+        <v>35</v>
+      </c>
+      <c r="G30">
+        <v>68</v>
+      </c>
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="11">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="E31" s="11">
+        <v>18</v>
+      </c>
+      <c r="F31">
+        <v>62</v>
+      </c>
+      <c r="G31">
+        <v>67</v>
+      </c>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="11">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11">
+        <v>19</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32">
+        <v>39</v>
+      </c>
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="11">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="11">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <v>43</v>
+      </c>
+      <c r="G33">
+        <v>28</v>
+      </c>
+      <c r="I33" s="11"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="11">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="I34" s="11"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="11">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="11">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="I36" s="11"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="11">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="11">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="11">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="11">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="11">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="I41" s="11"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="11">
+        <v>29</v>
+      </c>
+      <c r="B42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="I42" s="11"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="11">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="I43" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80035B98-A2A8-4D1B-8396-221B25D5B4C9}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3.4</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2.8</v>
+      </c>
+      <c r="C4">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2.9</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3.25</v>
+      </c>
+      <c r="C6">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>